<commit_message>
add LF in excel and python
</commit_message>
<xml_diff>
--- a/iir_llpf_calc.xlsx
+++ b/iir_llpf_calc.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{657BB1AD-D55E-F54F-9007-AC7AFD321510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8C7B84-7238-544C-9BC7-DDDB6AA39BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{2A289DFF-A98F-A740-AD45-78ACF3269FFD}"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{2A289DFF-A98F-A740-AD45-78ACF3269FFD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LPFz" sheetId="1" r:id="rId1"/>
+    <sheet name="LFz" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>cutoff freq</t>
   </si>
@@ -68,12 +69,6 @@
     <t>scale factor</t>
   </si>
   <si>
-    <t>b0_scale</t>
-  </si>
-  <si>
-    <t>b1_scale</t>
-  </si>
-  <si>
     <t>omega*T</t>
   </si>
   <si>
@@ -89,16 +84,71 @@
     <t xml:space="preserve">b1 </t>
   </si>
   <si>
-    <t>a1_scale</t>
+    <t>Single Pole Discrete Time IIR LPF</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Sample Time</t>
+  </si>
+  <si>
+    <t>Bilinear Z transform frequency pre-warp</t>
+  </si>
+  <si>
+    <t>Transfer function constants</t>
+  </si>
+  <si>
+    <t>Denominator</t>
+  </si>
+  <si>
+    <t>Numerator</t>
+  </si>
+  <si>
+    <t>b0_scaled</t>
+  </si>
+  <si>
+    <t>b1_scaled</t>
+  </si>
+  <si>
+    <t>a1_scaled</t>
+  </si>
+  <si>
+    <t>Proportional-Integral Loop Filter IIR</t>
+  </si>
+  <si>
+    <t>gain</t>
+  </si>
+  <si>
+    <t>tau 1</t>
+  </si>
+  <si>
+    <t>Gain normalizing time constant</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>usec</t>
+  </si>
+  <si>
+    <t>omega*T-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -125,8 +175,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,171 +494,457 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66D209-BD2F-6240-AA54-8860AB0744DA}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>1400</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>28800</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>28800</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <f>2*PI()*B2</f>
+        <v>8796.45943005142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>1/B3</f>
+        <v>3.4722222222222222E-5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>(2*B3)*TAN(B4*B5/2)</f>
+        <v>8865.4879330461536</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B6*B5</f>
+        <v>0.30782944211965813</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>2+(B8)</f>
+        <v>2.3078294421196581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>2-B8</f>
+        <v>1.6921705578803419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>B10/B9</f>
+        <v>0.7332303362618271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <f>B8/B9</f>
+        <v>0.13338483186908642</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f>B8/B9</f>
+        <v>0.13338483186908642</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f>POWER(2,B16)</f>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <f>ROUND(B17*B13,0)</f>
+        <v>4371</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <f>ROUND(B17*B14,0)</f>
+        <v>4371</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(B17*B12,0)</f>
+        <v>24026</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C83A625-5BAF-984C-8318-1E8337DD14A3}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
       <c r="B3">
-        <f>2*PI()*B1</f>
-        <v>8796.45943005142</v>
+        <v>28800</v>
       </c>
       <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>2*PI()*B2</f>
+        <v>879.64594300514204</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <f>1/B2</f>
+      <c r="B5">
+        <f>1/B3</f>
         <v>3.4722222222222222E-5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <f>(2*B2)*TAN(B3*B4/2)</f>
-        <v>8865.4879330461536</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B6">
+        <f>(2*B3)*TAN(B4*B5/2)</f>
+        <v>879.71433385608532</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <f>B5*B4</f>
-        <v>0.30782944211965813</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B6*B5</f>
+        <v>3.0545636592225183E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>2+(B8)</f>
+        <v>2.0305456365922252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <f>B8-2</f>
+        <v>-1.9694543634077748</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <f>1/(2*B6)</f>
+        <v>5.6836632160843731E-4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f>B11*1000000</f>
+        <v>568.36632160843726</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <f>2+(B7)</f>
-        <v>2.3078294421196581</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <f>B9</f>
+        <v>2.0305456365922252</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <f>2-B7</f>
-        <v>1.6921705578803419</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <f>B9/B8</f>
-        <v>0.7332303362618271</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <f>B7/B8</f>
-        <v>0.13338483186908642</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <f>B7/B8</f>
-        <v>0.13338483186908642</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B16">
+        <f>B10</f>
+        <v>-1.9694543634077748</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="B16">
-        <f>POWER(2,B15)</f>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <f>ROUND(B16*B12,0)</f>
-        <v>4371</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <f>ROUND(B16*B13,0)</f>
-        <v>4371</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
       <c r="B19">
-        <f>ROUND(B16*B11,0)</f>
-        <v>24026</v>
+        <f>POWER(2,B18)</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(B19*B15,0)</f>
+        <v>16634</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <f>ROUND(B16*B19,0)</f>
+        <v>-16134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <f>ROUND(B19*B14,0)</f>
+        <v>8192</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <f>1/(B11*B6*2)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved GFSK 9600 again
</commit_message>
<xml_diff>
--- a/iir_llpf_calc.xlsx
+++ b/iir_llpf_calc.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B733814-B960-BC4E-99A7-2143DE958479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DC0B4B-73F9-E342-A191-70560F10DFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{2A289DFF-A98F-A740-AD45-78ACF3269FFD}"/>
+    <workbookView xWindow="380" yWindow="1760" windowWidth="13800" windowHeight="15680" activeTab="2" xr2:uid="{2A289DFF-A98F-A740-AD45-78ACF3269FFD}"/>
   </bookViews>
   <sheets>
-    <sheet name="LPFz" sheetId="1" r:id="rId1"/>
-    <sheet name="LFz" sheetId="2" r:id="rId2"/>
+    <sheet name="LFz" sheetId="2" r:id="rId1"/>
+    <sheet name="LPFz LF" sheetId="3" r:id="rId2"/>
+    <sheet name="2nd order LPFz" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="36">
   <si>
     <t>cutoff freq</t>
   </si>
@@ -133,13 +134,25 @@
   </si>
   <si>
     <t>omega*T-2</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b2 scaled</t>
+  </si>
+  <si>
+    <t>a2 scaled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -153,6 +166,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,11 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,223 +513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66D209-BD2F-6240-AA54-8860AB0744DA}">
-  <dimension ref="A1:D20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1400</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>28800</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f>2*PI()*B2</f>
-        <v>8796.45943005142</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <f>1/B3</f>
-        <v>3.4722222222222222E-5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>8865.4879330461536</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <f>B6*B5</f>
-        <v>0.30782944211965813</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <f>2+(B8)</f>
-        <v>2.3078294421196581</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <f>2-B8</f>
-        <v>1.6921705578803419</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <f>B10/B9</f>
-        <v>0.7332303362618271</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <f>B8/B9</f>
-        <v>0.13338483186908642</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <f>B8/B9</f>
-        <v>0.13338483186908642</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17">
-        <f>POWER(2,B16)</f>
-        <v>32768</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <f>ROUND(B17*B13,0)</f>
-        <v>4371</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <f>ROUND(B17*B14,0)</f>
-        <v>4371</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <f>ROUND(B17*B12,0)</f>
-        <v>24026</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C83A625-5BAF-984C-8318-1E8337DD14A3}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>480</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -754,7 +562,7 @@
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>376.99111843077515</v>
+        <v>3015.9289474462012</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -781,7 +589,7 @@
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>376.99650155715949</v>
+        <v>3018.6880867031732</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -796,7 +604,7 @@
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>1.3090156304068038E-2</v>
+        <v>0.10481555856608241</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
@@ -808,7 +616,7 @@
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.013090156304068</v>
+        <v>2.1048155585660826</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -817,7 +625,7 @@
       </c>
       <c r="B10">
         <f>B8-2</f>
-        <v>-1.986909843695932</v>
+        <v>-1.8951844414339176</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -826,7 +634,7 @@
       </c>
       <c r="B11">
         <f>1/(2*B6)</f>
-        <v>1.3262722543439596E-3</v>
+        <v>1.6563486708097406E-4</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -838,7 +646,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12">
         <f>B11*1000000</f>
-        <v>1326.2722543439595</v>
+        <v>165.63486708097406</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -861,7 +669,7 @@
       </c>
       <c r="B15">
         <f>B9</f>
-        <v>2.013090156304068</v>
+        <v>2.1048155585660826</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
@@ -873,7 +681,7 @@
       </c>
       <c r="B16">
         <f>B10</f>
-        <v>-1.986909843695932</v>
+        <v>-1.8951844414339176</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
@@ -902,7 +710,7 @@
       </c>
       <c r="B20">
         <f>ROUND(B19*B15,0)</f>
-        <v>16491</v>
+        <v>17243</v>
       </c>
       <c r="D20" t="s">
         <v>20</v>
@@ -914,7 +722,7 @@
       </c>
       <c r="B21">
         <f>ROUND(B16*B19,0)</f>
-        <v>-16277</v>
+        <v>-15525</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
@@ -939,6 +747,464 @@
       <c r="B23">
         <f>1/(B11*B6*2)</f>
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D5EB82-167D-D34F-B315-B94EB3A2B45A}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>28800</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>2*PI()*B2</f>
+        <v>753.98223686155029</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>1/B3</f>
+        <v>3.4722222222222222E-5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>(2*B3)*TAN(B4*B5/2)</f>
+        <v>754.02530408650091</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B6*B5</f>
+        <v>2.618143416967017E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>2+(B8)</f>
+        <v>2.0261814341696702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>2-B8</f>
+        <v>1.9738185658303298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>B10/B9</f>
+        <v>0.97415687092168091</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <f>B8/B9</f>
+        <v>1.292156453915951E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <f>B8/B9</f>
+        <v>1.292156453915951E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <f>POWER(2,B16)</f>
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <f>ROUND(B17*B13,0)</f>
+        <v>423</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <f>ROUND(B17*B14,0)</f>
+        <v>423</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(B17*B12,0)</f>
+        <v>31921</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66D209-BD2F-6240-AA54-8860AB0744DA}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1400</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>28800</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>2*PI()*B2</f>
+        <v>8796.45943005142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>1/B3</f>
+        <v>3.4722222222222222E-5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>(2*B3)*TAN(B4*B5/2)</f>
+        <v>8865.4879330461536</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B6*B5</f>
+        <v>0.30782944211965813</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <f>2+(B8)</f>
+        <v>2.3078294421196581</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>2-B8</f>
+        <v>1.6921705578803419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>-1.5729712736308801</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.64930619341182005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f>1/52.4006576738302</f>
+        <v>1.9083729945233441E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>2/52.4006576738302</f>
+        <v>3.8167459890466882E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <f>1/52.4006576738302</f>
+        <v>1.9083729945233441E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <f>POWER(2,B18)</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <f>ROUND(B19*B14,0)</f>
+        <v>313</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <f>ROUND(B19*B15,0)</f>
+        <v>625</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22">
+        <f>ROUND(B19*B16,0)</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <f>ROUND(B19*B12,0)</f>
+        <v>-25772</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <f>ROUND(B19*B13,0)</f>
+        <v>10638</v>
       </c>
     </row>
   </sheetData>

</xml_diff>